<commit_message>
feat: adecuacion para mas de un feature
</commit_message>
<xml_diff>
--- a/feature_report.xlsx
+++ b/feature_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,17 +453,34 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>D:\IBK\Proyectos\documnetadorfeatures\CerrarSesion.feature</t>
+          <t>D:\IBK\Proyectos\documnetadorfeatures\test2\Login.feature</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['@PopupCerrarSesion', '@CLOSE_SESSION1']</t>
+          <t>['@Automated', '@Happy_path', '@Functional_testing', '@MilesRegression', '@regressionTest', '@LoginTest']</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[HAPPY PATH] Usuario espera primer popup y dar click en cerrar sesion</t>
+          <t>[HAPPY PATH] Validar el ingreso con diferentes tipo de documento - Usuario existente</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>D:\IBK\Proyectos\documnetadorfeatures\test2\Login.feature</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>['@Automated', '@Happy_path', '@Functional_testing', '@MilesRegression']</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[HAPPY PATH] Validar el ingreso a Mi cuenta</t>
         </is>
       </c>
     </row>

</xml_diff>